<commit_message>
task 40 dataset changed
</commit_message>
<xml_diff>
--- a/output/PSOchart.xlsx
+++ b/output/PSOchart.xlsx
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>19.1795</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>25.5727</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>13.5855</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>7.0303</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>23.4417</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>16.2493</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0</v>
+        <v>17.9394</v>
       </c>
       <c r="AK3" t="n">
         <v>0</v>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11.1576</v>
+        <v>18.174</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>19.8047</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>14.1116</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>25.3835</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>18.9679</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="n">
         <v>0</v>
@@ -884,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="AN4" t="n">
-        <v>0</v>
+        <v>11.1182</v>
       </c>
       <c r="AO4" t="n">
-        <v>11.9944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -903,16 +903,16 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>19.9264</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>11.2</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -945,10 +945,10 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="S5" t="n">
-        <v>17.3273</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>4.765</v>
+        <v>0</v>
       </c>
       <c r="AM5" t="n">
         <v>0</v>
@@ -1030,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>41.021</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>43.0917</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>35.5677</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -1093,10 +1093,10 @@
         <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>34.6399</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>38.3037</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1166,13 +1166,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>41.2371</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>53.8117</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>114.5475</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="AG7" t="n">
-        <v>0</v>
+        <v>19.7309</v>
       </c>
       <c r="AH7" t="n">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="AM7" t="n">
-        <v>0</v>
+        <v>52.0179</v>
       </c>
       <c r="AN7" t="n">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>19.9241</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1353,16 +1353,16 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>0.8038999999999999</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>75.56270000000001</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>24.6679</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>0</v>
+        <v>47.4277</v>
       </c>
       <c r="AJ8" t="n">
         <v>0</v>
@@ -1408,13 +1408,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>14.7887</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>38.4615</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1447,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0.7042</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>70.8899</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>69.38160000000001</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>30.2817</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
@@ -1480,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="AA9" t="n">
-        <v>58.4507</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>26.0563</v>
+        <v>0</v>
       </c>
       <c r="AJ9" t="n">
         <v>0</v>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.8811</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1559,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>12.6582</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>80.17619999999999</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1571,13 +1571,13 @@
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>68.7161</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>18.0832</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>24.6696</v>
       </c>
       <c r="Z10" t="n">
         <v>0</v>
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>71.6216</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>8.1081</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>32.4544</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -1716,10 +1716,10 @@
         <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>10.8181</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>52.7383</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
         <v>0</v>
@@ -1740,10 +1740,10 @@
         <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>43.2725</v>
+        <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>0</v>
+        <v>98.6486</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>29.4574</v>
+        <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>0</v>
+        <v>35.9053</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="AE12" t="n">
-        <v>0</v>
+        <v>42.7807</v>
       </c>
       <c r="AF12" t="n">
         <v>0</v>
@@ -1888,13 +1888,13 @@
         <v>0</v>
       </c>
       <c r="AJ12" t="n">
-        <v>18.6047</v>
+        <v>0</v>
       </c>
       <c r="AK12" t="n">
         <v>0</v>
       </c>
       <c r="AL12" t="n">
-        <v>0</v>
+        <v>33.6134</v>
       </c>
       <c r="AM12" t="n">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="AO12" t="n">
-        <v>0</v>
+        <v>61.8793</v>
       </c>
     </row>
     <row r="13">
@@ -1940,16 +1940,16 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>29.656</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>107.9478</v>
       </c>
       <c r="N13" t="n">
-        <v>48.8058</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
@@ -2000,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>67.4974</v>
+        <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>0</v>
+        <v>27.2835</v>
       </c>
       <c r="AG13" t="n">
         <v>0</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="AN13" t="n">
-        <v>30.1142</v>
+        <v>0</v>
       </c>
       <c r="AO13" t="n">
         <v>0</v>
@@ -2076,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>39.604</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>53.9054</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -2100,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>0</v>
+        <v>68.2068</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
@@ -2145,13 +2145,13 @@
         <v>0</v>
       </c>
       <c r="AK14" t="n">
-        <v>22.0472</v>
+        <v>0</v>
       </c>
       <c r="AL14" t="n">
         <v>0</v>
       </c>
       <c r="AM14" t="n">
-        <v>129.1339</v>
+        <v>0</v>
       </c>
       <c r="AN14" t="n">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>28.922</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>15.3846</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -2260,10 +2260,10 @@
         <v>0</v>
       </c>
       <c r="AG15" t="n">
-        <v>64.8554</v>
+        <v>0</v>
       </c>
       <c r="AH15" t="n">
-        <v>0</v>
+        <v>1.2821</v>
       </c>
       <c r="AI15" t="n">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="AK15" t="n">
-        <v>0</v>
+        <v>94.87179999999999</v>
       </c>
       <c r="AL15" t="n">
         <v>0</v>

</xml_diff>